<commit_message>
Tianyu Qi Diary 1/20/2020
</commit_message>
<xml_diff>
--- a/diaries/diary-tianyu-qi.xlsx
+++ b/diaries/diary-tianyu-qi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\code\SWE265P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\265P REVERSE_ENG_&amp;_MODEL\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F483857-DE8C-46D8-932A-AFAA489B9A82}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2DA025-0BB7-433B-8B3D-3143984B4FA8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="5760" yWindow="1284" windowWidth="17280" windowHeight="8964" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -54,42 +54,18 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
     <t>Reflection</t>
   </si>
   <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
     <t>Your Overall Mood</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
-    <t>Etc.</t>
-  </si>
-  <si>
     <t>Tianyu Qi</t>
   </si>
   <si>
@@ -105,16 +81,83 @@
     <t>5:00 - 7:50 pm</t>
   </si>
   <si>
-    <t>know what to expect in the course</t>
-  </si>
-  <si>
-    <t>learn course structure and set up working environments</t>
-  </si>
-  <si>
-    <t>this course is useful for furture work!</t>
-  </si>
-  <si>
-    <t>excited about coming classes</t>
+    <t>Know what to expect in the course</t>
+  </si>
+  <si>
+    <t>This course is useful for furture work!</t>
+  </si>
+  <si>
+    <t>Excited about coming classes</t>
+  </si>
+  <si>
+    <t>1/12/2020</t>
+  </si>
+  <si>
+    <t>10:00 - 1:00 am</t>
+  </si>
+  <si>
+    <t>(class)</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Build and run Java applications in different sizes to get more familir with IntelliJ IDEA</t>
+  </si>
+  <si>
+    <t>Learned course structure and set up working environments</t>
+  </si>
+  <si>
+    <t>1) Learned about some shortcuts in IntelliJ to navigate between files and code blocks quickly
+2) Installed some plug-ins from the marketplace</t>
+  </si>
+  <si>
+    <t>There are many more advanced tools/funtions to make coding and debugging easier and more interesting.</t>
+  </si>
+  <si>
+    <t>Can't wait to try what I've learnt</t>
+  </si>
+  <si>
+    <t>1/16/2020</t>
+  </si>
+  <si>
+    <t>5:00 - 8:05 pm</t>
+  </si>
+  <si>
+    <t>(class)
+Visitor: Ping Chen from Google</t>
+  </si>
+  <si>
+    <t>1) Learned basic strategies of reverse engineering
+2) Used the strategies to fix a bug and make changes to code (JPacMan1), learn the implementation of code (JPacMan2), and do code review and change functionality (JPacMan3)
+3) Enjoyed a great "interview" between Andre and Ping</t>
+  </si>
+  <si>
+    <t>It is not necessary to understand each line of code. We read code to solve problems, so solving problems is the goal. Double check before making any change. And focus on details.</t>
+  </si>
+  <si>
+    <t>Less afraid of reading code, but still nervous when meet bugs.</t>
+  </si>
+  <si>
+    <t>1/20/2020</t>
+  </si>
+  <si>
+    <t>5:00 - 6:30 pm</t>
+  </si>
+  <si>
+    <t>Start learning basic strategies and tools to do reverse engineering</t>
+  </si>
+  <si>
+    <t>Continue to explore JPacMan3 and finish the homework</t>
+  </si>
+  <si>
+    <t>Finished the homework</t>
+  </si>
+  <si>
+    <t>Clear and concise comments will greatly reduce the time of reviewing and changing code.</t>
+  </si>
+  <si>
+    <t>Good!</t>
   </si>
 </sst>
 </file>
@@ -253,7 +296,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,11 +322,23 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -605,34 +660,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" customWidth="1"/>
+    <col min="6" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -648,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -660,8 +720,8 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>20</v>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -673,8 +733,8 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>21</v>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -711,160 +771,172 @@
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="D11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G11" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>

</xml_diff>

<commit_message>
Tianyu Qi diary 1/29/2020
</commit_message>
<xml_diff>
--- a/diaries/diary-tianyu-qi.xlsx
+++ b/diaries/diary-tianyu-qi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\265P REVERSE_ENG_&amp;_MODEL\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2DA025-0BB7-433B-8B3D-3143984B4FA8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1BA0C0-BC2C-4024-8633-031223DAA6FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1284" windowWidth="17280" windowHeight="8964" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -158,6 +158,103 @@
   </si>
   <si>
     <t>Good!</t>
+  </si>
+  <si>
+    <t>1/23/2020</t>
+  </si>
+  <si>
+    <t>(class)
+Visitor: Alegria from ZocDoc</t>
+  </si>
+  <si>
+    <t>Learn Mental models and UML</t>
+  </si>
+  <si>
+    <t>1) Learned the conceps of mental models
+2) Externalized mental models with pen and paper
+3) Externalized mental models with UML
+4) Thanks Alegria for a wonderful sharing</t>
+  </si>
+  <si>
+    <t>The mental model templates seem tedious but do help! It's easy to feel lost in hundreds of files so it's necessary to keep track of the thinking flow. UML is a great tool for visualizing file relationships.</t>
+  </si>
+  <si>
+    <t>Pen and paper are still the best friends to read code. UML is so helpful but we should print them out and always make notes.</t>
+  </si>
+  <si>
+    <t>1/24/2020</t>
+  </si>
+  <si>
+    <t>build the project and run</t>
+  </si>
+  <si>
+    <t>Built the project following the document but failed to run it</t>
+  </si>
+  <si>
+    <t>Cannot figure out what was wrong</t>
+  </si>
+  <si>
+    <t>disappointed</t>
+  </si>
+  <si>
+    <t>1/27/2020</t>
+  </si>
+  <si>
+    <t>9:00 - 10:00 am</t>
+  </si>
+  <si>
+    <t>4:00 - 5:00 pm</t>
+  </si>
+  <si>
+    <t>Armin</t>
+  </si>
+  <si>
+    <t>Finish Feature 1</t>
+  </si>
+  <si>
+    <t>Failed to find the correct entry point for adding a table to Cassandra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry products are far more complicated than we expected considering its scalability and reliability. </t>
+  </si>
+  <si>
+    <t>disappointed again. Poor me.</t>
+  </si>
+  <si>
+    <t>1/28/2020</t>
+  </si>
+  <si>
+    <t>8:00 - 9:00 pm</t>
+  </si>
+  <si>
+    <t>Weihuan</t>
+  </si>
+  <si>
+    <t>Finish Feature 2</t>
+  </si>
+  <si>
+    <t>Found the implementation and even some code blocks related to feature 1.</t>
+  </si>
+  <si>
+    <t>Having an overall understanding of a product (differences Memtable and SSTable, and the "table" we think about) will help a lot in understanding codes.</t>
+  </si>
+  <si>
+    <t>finally a little excited about the homework</t>
+  </si>
+  <si>
+    <t>1/29/2020</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extended Armin's work after the work with Weihuan. </t>
+  </si>
+  <si>
+    <t>Industry products are COMPLICATED! Checking some related features may help understanding the feature we focus on.</t>
+  </si>
+  <si>
+    <t>Extended Feature 1</t>
   </si>
 </sst>
 </file>
@@ -296,7 +393,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -325,9 +422,6 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -337,7 +431,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -660,39 +769,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" customWidth="1"/>
-    <col min="6" max="7" width="34.6640625" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -783,160 +893,230 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12"/>
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>

</xml_diff>

<commit_message>
Tianyu Qi diary 2/5/2020
</commit_message>
<xml_diff>
--- a/diaries/diary-tianyu-qi.xlsx
+++ b/diaries/diary-tianyu-qi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\265P REVERSE_ENG_&amp;_MODEL\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1BA0C0-BC2C-4024-8633-031223DAA6FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBA4D25-C2FD-41C6-9558-824698A42004}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="7476" yWindow="372" windowWidth="15372" windowHeight="11388" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -254,14 +254,85 @@
     <t>Industry products are COMPLICATED! Checking some related features may help understanding the feature we focus on.</t>
   </si>
   <si>
-    <t>Extended Feature 1</t>
+    <t>1/30/2020</t>
+  </si>
+  <si>
+    <t>(class)
+Visitor: Consuelo Lopez</t>
+  </si>
+  <si>
+    <t>Learn about key expert practices in reading code, differences between structural and behavioral models, and practice more about UML</t>
+  </si>
+  <si>
+    <t>1) Know the three KEPs and try to implement them in in-class practices
+2) Learned from a real example of Mirth 
+3) UML class diagram notations
+4) Two new tools: call graphs and sequence diagram</t>
+  </si>
+  <si>
+    <t>It is critical to understand what the code really does. Make both structural and behavioral models will help. It does not have to be formal and precise, the content they convey is more crutial. 
+There are more to discover in UML from the notations.</t>
+  </si>
+  <si>
+    <t>2/2/2020</t>
+  </si>
+  <si>
+    <t>10:00 am -1:00 pm</t>
+  </si>
+  <si>
+    <t>Weihuan and Armin</t>
+  </si>
+  <si>
+    <t>Successfully found how to assgin permissions! Found the exace query!</t>
+  </si>
+  <si>
+    <t>Satisfied!</t>
+  </si>
+  <si>
+    <t>2/3/2020</t>
+  </si>
+  <si>
+    <t>1:30 - 2:30 pm</t>
+  </si>
+  <si>
+    <t>Kaj and Weihuan</t>
+  </si>
+  <si>
+    <t>It finally worked!</t>
+  </si>
+  <si>
+    <t>You learn from making mistakes.I'll never make the same mistake again.</t>
+  </si>
+  <si>
+    <t>Happy! Thanks Kaj!</t>
+  </si>
+  <si>
+    <t>2:30 - 4:30 pm</t>
+  </si>
+  <si>
+    <t>Extend Feature 1</t>
+  </si>
+  <si>
+    <t>Build the source code</t>
+  </si>
+  <si>
+    <t>Sucessfully figured out how the query is parsed and executed</t>
+  </si>
+  <si>
+    <t>The hard thing is always to find a feature. After that, you just follow the code and see.</t>
+  </si>
+  <si>
+    <t>Great!</t>
+  </si>
+  <si>
+    <t>Choose a feature that is very specific will help a lot in understanding it. Use the graphs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +424,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -393,7 +506,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -419,9 +532,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -430,9 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -449,6 +556,23 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -769,14 +893,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B122" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="21" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" customWidth="1"/>
     <col min="5" max="5" width="39.6640625" customWidth="1"/>
@@ -785,28 +909,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -830,7 +954,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
@@ -843,7 +967,7 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1"/>
@@ -854,7 +978,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -863,7 +987,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -874,7 +998,7 @@
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -893,257 +1017,313 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:7" s="11" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:7" s="11" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:7" s="11" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:7" s="14" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="16" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:7" s="14" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="22" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="11" t="s">
+      <c r="B19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
@@ -2072,6 +2252,6 @@
     <hyperlink ref="B6" r:id="rId2" xr:uid="{EDFFD169-F81E-4158-82D9-737A15A0D1A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tianyu Qi diary 2/19/2020
</commit_message>
<xml_diff>
--- a/diaries/diary-tianyu-qi.xlsx
+++ b/diaries/diary-tianyu-qi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBA4D25-C2FD-41C6-9558-824698A42004}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6991484-784A-4A52-9D6C-1B35271D2B90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7476" yWindow="372" windowWidth="15372" windowHeight="11388" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="9516" yWindow="1248" windowWidth="15372" windowHeight="11388" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="130">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>10:00 - 1:00 am</t>
-  </si>
-  <si>
-    <t>(class)</t>
   </si>
   <si>
     <t>/</t>
@@ -122,10 +119,6 @@
   </si>
   <si>
     <t>5:00 - 8:05 pm</t>
-  </si>
-  <si>
-    <t>(class)
-Visitor: Ping Chen from Google</t>
   </si>
   <si>
     <t>1) Learned basic strategies of reverse engineering
@@ -161,10 +154,6 @@
   </si>
   <si>
     <t>1/23/2020</t>
-  </si>
-  <si>
-    <t>(class)
-Visitor: Alegria from ZocDoc</t>
   </si>
   <si>
     <t>Learn Mental models and UML</t>
@@ -257,10 +246,6 @@
     <t>1/30/2020</t>
   </si>
   <si>
-    <t>(class)
-Visitor: Consuelo Lopez</t>
-  </si>
-  <si>
     <t>Learn about key expert practices in reading code, differences between structural and behavioral models, and practice more about UML</t>
   </si>
   <si>
@@ -326,6 +311,140 @@
   </si>
   <si>
     <t>Choose a feature that is very specific will help a lot in understanding it. Use the graphs.</t>
+  </si>
+  <si>
+    <t>(Lecture 1)</t>
+  </si>
+  <si>
+    <t>(Lecture 2)
+Visitor: Ping Chen from Google</t>
+  </si>
+  <si>
+    <t>(Lecture 3)
+Visitor: Alegria from ZocDoc</t>
+  </si>
+  <si>
+    <t>(Lecture 4)
+Visitor: Consuelo Lopez</t>
+  </si>
+  <si>
+    <t>Learn about more key expert practices in reading code, and mental simulation</t>
+  </si>
+  <si>
+    <t>(Lecture 5)
+Visitor: Christopher Keller</t>
+  </si>
+  <si>
+    <t>1) Reflected on the first three key expert practices and learnd three more
+2) The 4th important frequent question
+3) Learned the concepts about mental simulation and practiced in class with "Hello word" and "Hello world" examples
+4) JPacMan practices</t>
+  </si>
+  <si>
+    <t>Two of the three new KEPs (simulate continually and draw examples alongside their diagrams) are talking about the same thing: try it, instead of just think about it. I always refuse to write and draw when solving coding problems (because of laziness) but I should change my way. Pen and paper tells me if I really understand, not the debugger.</t>
+  </si>
+  <si>
+    <t>2/6/2020</t>
+  </si>
+  <si>
+    <t>Great! No homework!</t>
+  </si>
+  <si>
+    <t>2/9/2020</t>
+  </si>
+  <si>
+    <t>Summarize concepts for midterm</t>
+  </si>
+  <si>
+    <t>A markdown file of 5 pages full of concepts and graphs</t>
+  </si>
+  <si>
+    <t>There are a lot we learned and a lot I already forgot. I do not like exams but it helps to reflect on the achievements so far.</t>
+  </si>
+  <si>
+    <t>A sense of achievement!</t>
+  </si>
+  <si>
+    <t>2/12/2020
+2/13/2020</t>
+  </si>
+  <si>
+    <t>10:00 - 11:00pm
+3:00 - 5:00 pm</t>
+  </si>
+  <si>
+    <t>1:30 - 4:30 pm</t>
+  </si>
+  <si>
+    <t>We will see from the exam result.</t>
+  </si>
+  <si>
+    <t>Recite and understand concepts</t>
+  </si>
+  <si>
+    <t>Come to understand why we should have this exam. We learned a lot but without remembering the concepts, it is hard to express ourselves clearly. If we fail to express well, it is the same as we did not learn (well), from others' percepectives.</t>
+  </si>
+  <si>
+    <t>Thanks Andre!</t>
+  </si>
+  <si>
+    <t>2/13/2020</t>
+  </si>
+  <si>
+    <t>More key expert practices and what to look at when we talk about the big picture of a project</t>
+  </si>
+  <si>
+    <t>midterm
+(Lecture 6)</t>
+  </si>
+  <si>
+    <t>2/16/2020</t>
+  </si>
+  <si>
+    <t>1) Learned three new key expert practices
+2) Learned about new angles to describe a project: stakeholders, key developers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This class inspires me to see a project from the stakeholders' perspectives. We want to make good programs for our customers/users, so we should think more from their angles instead of focusing only on the implementation. </t>
+  </si>
+  <si>
+    <t>2:00 - 5:00 pm</t>
+  </si>
+  <si>
+    <t>Finish most of the assignment.</t>
+  </si>
+  <si>
+    <t>Figured out the major stakeholders and top contributors of the project. Went through the open issues and tried to understand the problems.</t>
+  </si>
+  <si>
+    <t>It turned out going through the open issues is another way to learn more about the project. Users talked about the scenarios in which they use the product and how they think about it when they open issues.</t>
+  </si>
+  <si>
+    <t>Happy about the progress!</t>
+  </si>
+  <si>
+    <t>2/19/2020</t>
+  </si>
+  <si>
+    <t>10:00 - 11:00pm</t>
+  </si>
+  <si>
+    <t>Finalize the assignment for this week.</t>
+  </si>
+  <si>
+    <t>Changed some contents about essential functional aspects and essential non-functional aspects about the project.</t>
+  </si>
+  <si>
+    <t>"Essential functional = actual functionality that the system offers (e.g., store data,  access data quickly, create reports)
+Non-essential functionality = other properties of the system (e.g., secure,  fault-tolerant,maintainable, evolvable, usable, ...)
+more driven by 'crosscutting concerns about the state of the system overall'." - Andre</t>
+  </si>
+  <si>
+    <t>2/20/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Lecture 7)
+</t>
   </si>
 </sst>
 </file>
@@ -506,7 +625,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,9 +675,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -572,7 +688,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -893,14 +1011,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B122" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="20" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" customWidth="1"/>
     <col min="5" max="5" width="39.6640625" customWidth="1"/>
@@ -909,28 +1027,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="18"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -954,7 +1072,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
@@ -967,7 +1085,7 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1"/>
@@ -978,7 +1096,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="18"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -998,7 +1116,7 @@
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1025,13 +1143,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>17</v>
@@ -1048,332 +1166,422 @@
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="E11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="11" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="G12" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="G13" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="11" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="G14" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="G15" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="D16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="G16" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="E17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="F17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="G17" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="14" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="G18" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="21" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="22" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="21" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="B20" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="D20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="22" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="F20" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="G21" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="9" t="s">
+    </row>
+    <row r="22" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="C22" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="G22" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="21" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="11" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="11" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="11" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="11" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>

</xml_diff>

<commit_message>
Tianyu Qi diary 3/5/2020
</commit_message>
<xml_diff>
--- a/diaries/diary-tianyu-qi.xlsx
+++ b/diaries/diary-tianyu-qi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tianyu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6991484-784A-4A52-9D6C-1B35271D2B90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A43F977-9C14-4D6A-9A6E-0A83FC852678}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9516" yWindow="1248" windowWidth="15372" windowHeight="11388" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="168">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -443,8 +443,132 @@
     <t>2/20/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">(Lecture 7)
-</t>
+    <t>(Lecture 7)
+Visitor: Sara and Omar</t>
+  </si>
+  <si>
+    <t>More KEPs, also architecture and social context of the project</t>
+  </si>
+  <si>
+    <t>2/21/2020</t>
+  </si>
+  <si>
+    <t>2/23/2020</t>
+  </si>
+  <si>
+    <t>2/25/2020</t>
+  </si>
+  <si>
+    <t>9:00 - 11:30pm</t>
+  </si>
+  <si>
+    <t>1:00 - 5:30pm
+7:00 - 10:00pm</t>
+  </si>
+  <si>
+    <t>8:00 - 11:00pm</t>
+  </si>
+  <si>
+    <t>2/27/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish homework: Architecture </t>
+  </si>
+  <si>
+    <t>Finally!</t>
+  </si>
+  <si>
+    <t>1) Three more KEPs
+2) Concepts about project architecture, and how to do architecture recovery, practice with JPacman
+3) What are the social context of a project
+4) code review ideally and in reality</t>
+  </si>
+  <si>
+    <t>KEPs for this week are telling me to be proactive. BE PROACTIVE, to learn backgound knowledge, know how things work, and design elegantly. The JPacman practice is really helpful in learning architecture recovery. I will try using it in doing the homework.</t>
+  </si>
+  <si>
+    <t>Try to find a documented architecture.</t>
+  </si>
+  <si>
+    <t>Failed to find one.</t>
+  </si>
+  <si>
+    <t>This is hard. Need to plan more time in this.</t>
+  </si>
+  <si>
+    <t>Even if it's famous and widely-used, there is no good documentation about the architecture. And many articles named with "Cassandra Architecture" are just copying from each other!</t>
+  </si>
+  <si>
+    <t>Changed to find architecutre of "database" instead of "Cassandra", and followed that route to see Cassandra codebase from a different way. Failed to finish, but knew what to plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The KEP: do something else, works! Also, when you get stuck in one place, look around and look into the bigger picture. Database architecture gives me us a clue to check the Cassandra codebase and the tast changes from reverse-engineering the architecture to validate that. </t>
+  </si>
+  <si>
+    <t>Tired!</t>
+  </si>
+  <si>
+    <t>Finish 1st pull request</t>
+  </si>
+  <si>
+    <t>10:00 - 11:00am</t>
+  </si>
+  <si>
+    <t>Made the FIRST contribution to Cassandra.</t>
+  </si>
+  <si>
+    <t>(Lecture 8)
+Visitor: Alberto</t>
+  </si>
+  <si>
+    <t>9:00am - 12:00pm</t>
+  </si>
+  <si>
+    <t>Find two design patterns.</t>
+  </si>
+  <si>
+    <t>Three more KEPs, testing and in-class testing practice.</t>
+  </si>
+  <si>
+    <t>Summarized the thinking process and organized words to finish the report.</t>
+  </si>
+  <si>
+    <t>Make more notes, add webpages to favorite in the browser, and keep screenshots help to write a report.</t>
+  </si>
+  <si>
+    <t>More KEPs and design patterns (concept, categories, examples)</t>
+  </si>
+  <si>
+    <t>1) Three more KEPs
+2) Design patterns with the Duck example.</t>
+  </si>
+  <si>
+    <t>Love the KEP: use analogy. If we can use simple daily examples to describe and explain the code logic or differences between parts, we must really understand it. There are a LOT of design patterns which can save us plenty of time. Interested to discover more after class.</t>
+  </si>
+  <si>
+    <t>Finished with Singleton and Builder.</t>
+  </si>
+  <si>
+    <t>I wrote too few projects that I do not even have a chance to use these two common patterns. Wanna try.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be brave! </t>
+  </si>
+  <si>
+    <t>(Lecture 9)
+Visitor: Eric and Michael</t>
+  </si>
+  <si>
+    <t>1) Learned about how other groups submit their pull requests. Got some inspirations.
+2) Three more KEPs. 
+3) Testing concepts, tactics, and practice with JPacMan4 tests.</t>
+  </si>
+  <si>
+    <t>Testing part complements Prof. Jones' class with hands-on pratice in discovering existing test cases. 
+Enjoyed the lecture from Eric and Michael! They are the kind of computer scientists we dream to be!</t>
   </si>
 </sst>
 </file>
@@ -625,7 +749,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -687,6 +811,15 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1011,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,31 +1153,31 @@
     <col min="1" max="1" width="17.109375" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" style="20" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
     <col min="5" max="5" width="39.6640625" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
     <col min="7" max="7" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1572,110 +1705,216 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:7" s="11" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
+      <c r="D29" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="11" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="11" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="11" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="24" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="22">
+        <v>43891</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="24" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="22">
+        <v>43893</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="24" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="22">
+        <v>43895</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>

</xml_diff>